<commit_message>
Fixed error in file naming.
</commit_message>
<xml_diff>
--- a/NCAA_Games.xlsx
+++ b/NCAA_Games.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\Desktop\PythonProjects\DraftPredictions\bracket-predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E3AF7D3-B5F0-4FF0-A3E4-B37943EBDA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3EB04D-DD9A-4647-AD32-28A940565302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="195" windowWidth="17205" windowHeight="14610" xr2:uid="{064EBF74-BDD8-4B7E-BC44-E231380FA68E}"/>
+    <workbookView xWindow="13185" yWindow="-18540" windowWidth="17880" windowHeight="16455" xr2:uid="{064EBF74-BDD8-4B7E-BC44-E231380FA68E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,15 +210,6 @@
     <t>Colorado</t>
   </si>
   <si>
-    <t>Grambling</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Howard</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -226,6 +217,15 @@
   </si>
   <si>
     <t>Num</t>
+  </si>
+  <si>
+    <t>Wagner</t>
+  </si>
+  <si>
+    <t>Colorado St.</t>
+  </si>
+  <si>
+    <t>Grambling St.</t>
   </si>
 </sst>
 </file>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6D37B5-B071-4550-981F-76FDAC92BC95}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +590,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
         <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>